<commit_message>
PROS-14717 LionJP Template validation
</commit_message>
<xml_diff>
--- a/Projects/LIONJP_SAND/Data/kpi_template.xlsx
+++ b/Projects/LIONJP_SAND/Data/kpi_template.xlsx
@@ -11,10 +11,18 @@
     <sheet name="kpi_config" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">kpi_config!$A$2:$O$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">kpi_config!$A$2:$O$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="74">
   <si>
     <t xml:space="preserve">LionJP</t>
   </si>
@@ -70,7 +78,7 @@
     <t xml:space="preserve">include_other_ean_codes</t>
   </si>
   <si>
-    <t xml:space="preserve">start_date1</t>
+    <t xml:space="preserve">start_date</t>
   </si>
   <si>
     <t xml:space="preserve">end_date</t>
@@ -124,12 +132,12 @@
     <t xml:space="preserve">Brand_Other_0001</t>
   </si>
   <si>
+    <t xml:space="preserve">12/31/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">HagukiPlus TP &amp; HagukiPlus Premium TP are HOR ADJ</t>
   </si>
   <si>
-    <t xml:space="preserve">include1</t>
-  </si>
-  <si>
     <t xml:space="preserve">4903301293064, 4903301293101, 4903301293088, 4903301293125</t>
   </si>
   <si>
@@ -148,9 +156,6 @@
     <t xml:space="preserve">Nonio TP &amp; Nonio Plus TP are HOR ADJ</t>
   </si>
   <si>
-    <t xml:space="preserve">product1</t>
-  </si>
-  <si>
     <t xml:space="preserve">4903301259299, 4903301259305, 4903301259312, 4903301268352, 4903301268369, 4903301268376, 4903301283751, 4903301283768, 4903301283775, 4903301297246, 4903301297253, 4903301297291, 4903301308904, 4903301300496</t>
   </si>
   <si>
@@ -163,66 +168,66 @@
     <t xml:space="preserve">DentHealth Non-Med TP &amp; Med TP are HOR ADJ</t>
   </si>
   <si>
+    <t xml:space="preserve">4903301136385, 4903301136392, 4903301136842, 4903301136859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand_Other_0004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinica AD TB &amp; NS TB are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301186359, 4903301186366, 4903301186373, 4903301186380, 4903301216148, 4903301216155, 4903301246985, 4903301246992, 4903301247005, 4903301247012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301283782, 4903301283799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systema TB &amp; Systema HagukiPlus TB are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301328469, 4903301328476, 4903301263944, 4903301263951, 4903301263968, 4903301263975, 4903301264033, 4903301264040, 4903301264064, 4903301264071, 4903301264088, 4903301282266, 4903301282273, 4903301294641, 4903301294719, 4903301294726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301274254, 4903301274247, 4903301274278, 4903301274261, 4903301274292, 4903301274285, 4903301290131, 4903301290148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systema TB &amp; Systema Ultrasonic TB are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301216247, 4903301129714, 4903301143970, 4903301129646, 4903301277125, 4903301144229, 4903301144236, 4903301222460, 4903301222477, 4903301290179, 4903301290193, 4903301299875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HagukiPlus TB &amp; Systema Ultrasonic TB are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinica AD TP &amp; NS TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systema EX TP &amp; Systema HagukiPlus TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HagukiPlus TP &amp; HagukiPlus Premium TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HagukiPlus TP &amp; DentHealth TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HagukiPlus Premium TP &amp; DentHealth TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonio TP &amp; Nonio Plus TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DentHealth Non-Med TP &amp; Med TP are VER ADJ</t>
+  </si>
+  <si>
     <t xml:space="preserve">4903301136385, 4903301136392, 4903301136842, 4903301136859, 4903301137559</t>
   </si>
   <si>
-    <t xml:space="preserve">Brand_Other_0004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinica AD TB &amp; NS TB are HOR ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4903301186359, 4903301186366, 4903301186373, 4903301186380, 4903301216148, 4903301216155, 4903301246985, 4903301246992, 4903301247005, 4903301247012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4903301283782, 4903301283799</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systema TB &amp; Systema HagukiPlus TB are HOR ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4903301328469, 4903301328476, 4903301263944, 4903301263951, 4903301263968, 4903301263975, 4903301264033, 4903301264040, 4903301264064, 4903301264071, 4903301264088, 4903301282266, 4903301282273, 4903301294641, 4903301294719, 4903301294726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4903301274254, 4903301274247, 4903301274278, 4903301274261, 4903301274292, 4903301274285, 4903301290131, 4903301290148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systema TB &amp; Systema Ultrasonic TB are HOR ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4903301216247, 4903301129714, 4903301143970, 4903301129646, 4903301277125, 4903301144229, 4903301144236, 4903301222460, 4903301222477, 4903301290179, 4903301290193, 4903301299875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HagukiPlus TB &amp; Systema Ultrasonic TB are HOR ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinica AD TP &amp; NS TP are VER ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systema EX TP &amp; Systema HagukiPlus TP are VER ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HagukiPlus TP &amp; HagukiPlus Premium TP are VER ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HagukiPlus TP &amp; DentHealth TP are VER ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HagukiPlus Premium TP &amp; DentHealth TP are VER ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonio TP &amp; Nonio Plus TP are VER ADJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DentHealth Non-Med TP &amp; Med TP are VER ADJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clinica AD TB &amp; NS TB are VER ADJ</t>
   </si>
   <si>
@@ -233,6 +238,9 @@
   </si>
   <si>
     <t xml:space="preserve">HagukiPlus TB &amp; Systema Ultrasonic TB are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand_Other_000112</t>
   </si>
   <si>
     <r>
@@ -536,33 +544,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:26"/>
+  <dimension ref="1:28"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,7 +1648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1692,7 +1700,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>18</v>
@@ -1719,13 +1727,13 @@
         <v>22</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>26</v>
@@ -1739,7 +1747,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>18</v>
@@ -1754,7 +1762,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>21</v>
@@ -1766,10 +1774,10 @@
         <v>22</v>
       </c>
       <c r="K5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>31</v>
@@ -1778,7 +1786,7 @@
         <v>26</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,7 +1794,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>18</v>
@@ -1813,13 +1821,13 @@
         <v>22</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>26</v>
@@ -1833,7 +1841,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
@@ -1860,13 +1868,13 @@
         <v>22</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>26</v>
@@ -1880,7 +1888,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>18</v>
@@ -1901,19 +1909,19 @@
         <v>21</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>26</v>
@@ -1927,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
@@ -1954,13 +1962,13 @@
         <v>22</v>
       </c>
       <c r="K9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>46</v>
+      <c r="M9" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>26</v>
@@ -1974,7 +1982,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>18</v>
@@ -2001,13 +2009,13 @@
         <v>22</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>26</v>
@@ -2021,7 +2029,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>18</v>
@@ -2039,7 +2047,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>22</v>
@@ -2048,13 +2056,13 @@
         <v>22</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>26</v>
@@ -2068,7 +2076,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>18</v>
@@ -2083,7 +2091,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>21</v>
@@ -2095,13 +2103,13 @@
         <v>22</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>26</v>
@@ -2115,7 +2123,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -2142,10 +2150,10 @@
         <v>22</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>31</v>
@@ -2162,13 +2170,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>40</v>
@@ -2189,13 +2197,13 @@
         <v>22</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="N14" s="6" t="s">
         <v>26</v>
@@ -2209,13 +2217,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>40</v>
@@ -2236,10 +2244,10 @@
         <v>22</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>31</v>
@@ -2256,13 +2264,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>40</v>
@@ -2283,13 +2291,13 @@
         <v>22</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>26</v>
@@ -2303,13 +2311,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>40</v>
@@ -2330,13 +2338,13 @@
         <v>22</v>
       </c>
       <c r="K17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="M17" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>26</v>
@@ -2350,13 +2358,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>40</v>
@@ -2377,13 +2385,13 @@
         <v>22</v>
       </c>
       <c r="K18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="M18" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>26</v>
@@ -2397,13 +2405,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>40</v>
@@ -2424,13 +2432,13 @@
         <v>22</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>26</v>
@@ -2444,13 +2452,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>40</v>
@@ -2471,13 +2479,13 @@
         <v>22</v>
       </c>
       <c r="K20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>46</v>
+      <c r="M20" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>26</v>
@@ -2491,13 +2499,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>40</v>
@@ -2518,13 +2526,13 @@
         <v>22</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>26</v>
@@ -2538,13 +2546,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>40</v>
@@ -2565,13 +2573,13 @@
         <v>22</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>31</v>
+        <v>63</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>26</v>
@@ -2585,13 +2593,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>40</v>
@@ -2612,13 +2620,13 @@
         <v>22</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="N23" s="6" t="s">
         <v>26</v>
@@ -2632,13 +2640,13 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>40</v>
@@ -2659,10 +2667,10 @@
         <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>31</v>
@@ -2679,13 +2687,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>40</v>
@@ -2706,12 +2714,14 @@
         <v>22</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M25" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="N25" s="6" t="s">
         <v>26</v>
       </c>
@@ -2724,13 +2734,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>40</v>
@@ -2751,12 +2761,14 @@
         <v>22</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="M26" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="N26" s="6" t="s">
         <v>26</v>
       </c>
@@ -2764,8 +2776,98 @@
         <v>27</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:O26"/>
+  <autoFilter ref="A2:O28"/>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updates: Data overlap checks based on report_label column, invalid dataformat checks added
</commit_message>
<xml_diff>
--- a/Projects/LIONJP_SAND/Data/kpi_template.xlsx
+++ b/Projects/LIONJP_SAND/Data/kpi_template.xlsx
@@ -5,24 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="kpi_config" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="75">
   <si>
     <t xml:space="preserve">LionJP</t>
   </si>
@@ -118,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">12/31/2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/02/2020</t>
   </si>
   <si>
     <t xml:space="preserve">Systema EX TP &amp; Systema HagukiPlus TP are HOR ADJ</t>
@@ -544,33 +536,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O6" activeCellId="0" sqref="O6"/>
+      <selection pane="bottomRight" activeCell="O4" activeCellId="0" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.71938775510204"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="46.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="9.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1731,7 @@
         <v>26</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,7 +1739,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>18</v>
@@ -1774,19 +1766,19 @@
         <v>22</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,7 +1786,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>18</v>
@@ -1821,13 +1813,13 @@
         <v>22</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>26</v>
@@ -1841,7 +1833,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
@@ -1868,13 +1860,13 @@
         <v>22</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>26</v>
@@ -1888,7 +1880,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>18</v>
@@ -1915,13 +1907,13 @@
         <v>22</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>26</v>
@@ -1935,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
@@ -1962,13 +1954,13 @@
         <v>22</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>26</v>
@@ -1982,7 +1974,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>18</v>
@@ -2009,13 +2001,13 @@
         <v>22</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>26</v>
@@ -2029,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>18</v>
@@ -2056,13 +2048,13 @@
         <v>22</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>26</v>
@@ -2076,7 +2068,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>18</v>
@@ -2103,10 +2095,10 @@
         <v>22</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>25</v>
@@ -2123,7 +2115,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -2150,13 +2142,13 @@
         <v>22</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>26</v>
@@ -2170,7 +2162,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>18</v>
@@ -2197,13 +2189,13 @@
         <v>22</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N14" s="6" t="s">
         <v>26</v>
@@ -2217,7 +2209,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>18</v>
@@ -2244,13 +2236,13 @@
         <v>22</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>26</v>
@@ -2264,13 +2256,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>40</v>
@@ -2311,13 +2303,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>40</v>
@@ -2338,13 +2330,13 @@
         <v>22</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>26</v>
@@ -2358,13 +2350,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>40</v>
@@ -2385,13 +2377,13 @@
         <v>22</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>26</v>
@@ -2405,13 +2397,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>40</v>
@@ -2432,13 +2424,13 @@
         <v>22</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>26</v>
@@ -2452,13 +2444,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>40</v>
@@ -2479,13 +2471,13 @@
         <v>22</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>26</v>
@@ -2499,13 +2491,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>40</v>
@@ -2526,13 +2518,13 @@
         <v>22</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>26</v>
@@ -2546,13 +2538,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>40</v>
@@ -2573,13 +2565,13 @@
         <v>22</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>26</v>
@@ -2593,13 +2585,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>40</v>
@@ -2620,10 +2612,10 @@
         <v>22</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>25</v>
@@ -2640,13 +2632,13 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>40</v>
@@ -2667,13 +2659,13 @@
         <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N24" s="6" t="s">
         <v>26</v>
@@ -2687,13 +2679,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>40</v>
@@ -2714,13 +2706,13 @@
         <v>22</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N25" s="6" t="s">
         <v>26</v>
@@ -2734,13 +2726,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>40</v>
@@ -2761,13 +2753,13 @@
         <v>22</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>26</v>
@@ -2781,13 +2773,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>40</v>
@@ -2808,10 +2800,10 @@
         <v>22</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="6" t="s">
@@ -2826,13 +2818,13 @@
         <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>40</v>
@@ -2853,10 +2845,10 @@
         <v>22</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="6" t="s">
@@ -2873,7 +2865,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
PROS-14717 lionjp adjacenty kpi cleanup and template validation
</commit_message>
<xml_diff>
--- a/Projects/LIONJP_SAND/Data/kpi_template.xlsx
+++ b/Projects/LIONJP_SAND/Data/kpi_template.xlsx
@@ -5,13 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="kpi_config" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="kpi_config_client" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="kpi_config_backup" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="kpi_config" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config_client!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config_client!$A$2:$O$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">kpi_config_client!$A$2:$O$28</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="113">
   <si>
     <t xml:space="preserve">LionJP</t>
   </si>
@@ -143,6 +147,9 @@
   </si>
   <si>
     <t xml:space="preserve">HagukiPlus Premium TP &amp; DentHealth TP are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Oral Care1</t>
   </si>
   <si>
     <t xml:space="preserve">Nonio TP &amp; Nonio Plus TP are HOR ADJ</t>
@@ -303,6 +310,117 @@
   <si>
     <t xml:space="preserve">4987643120059, 4987643121056, 4987643121063, 4987643122077, 4987643122084, 4987643122107, 4987643120066, 4987643122145, 4901301335678, 4901301337870, 4901301348975, 4901301351333, 4901301361721, 4901301382016, 4901301382023, 4901301382030</t>
   </si>
+  <si>
+    <t xml:space="preserve">5/25/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubCat Hanyo Bihaku &amp; mouthwash are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubCat Mouthwash, HE white &amp; Beauty are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horizontal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301241430, 4903301241447, 4903301241454, 4903301260714, 4903301260721, 4903301260738, 4903301271765, 4903301271772, 4903301271802 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/25/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301268871, 4903301268925, 4903301281511, 4903301281528, 4903301268963, 4903301268970, 4903301293781, 4903301297772, 4903301300878 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301216803, 4903301231073, 4903301231097, 4903301281559, 4903301281566, 4903301281573, 4903301277057, 4903301277064, 4903301277071, 4903301297734, 4903301297741, 4903301297765 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301293064, 4903301293101, 4903301293088, 4903301293125 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301259299, 4903301259305, 4903301259312, 4903301268352, 4903301268369, 4903301268376, 4903301283751, 4903301283768, 4903301283775, 4903301297246, 4903301297253, 4903301297291, 4903301308904, 4903301300496 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301248941, 4903301248958, 4903301249016, 4903301249023, 4903301249047, 4903301249061, 4903301275985, 4903301276005, 4903301248996, 4903301249030, 4903301249078, 4903301276012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301186359, 4903301186366, 4903301186373, 4903301186380, 4903301216148, 4903301216155, 4903301246985, 4903301246992, 4903301247005, 4903301247012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301328469, 4903301328476, 4903301263944, 4903301263951, 4903301263968, 4903301263975, 4903301264033, 4903301264040, 4903301264064, 4903301264071, 4903301264088, 4903301282266, 4903301282273, 4903301294641, 4903301294719, 4903301294726 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301274254, 4903301274247, 4903301274278, 4903301274261, 4903301274292, 4903301274285, 4903301290131, 4903301290148 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301259299, 4903301259305, 4903301259312, 4901616010543, 4901616010550, 4901616010635, 4901616010703, 4901616011410, 4903301268352, 4903301268369, 4903301268376, 4903301283751, 4903301283768, 4903301283775, 4903301293149, 4903301297246, 4903301297253, 4903301297291, 4903301293156, 4903301308904, 4903301300496 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubCat Mouthwash HE white &amp; Beauty are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4977545315660, 4533213090583, 4543268057066, 4543268066587, 4571138552823, 4582469494713, 4582469494720, 4901301307828, 4571138552816, 4573350880265, 4987107624154, 4987107624161, 4992440034911, 4543268071192, 4533213670105, 4582469503002, 4901301367334, 4901301367600, 4901301368058, 4560452210373, 4571407930185, 4582252821061, 4543268078344, 4541189007085, 4988439005772, 4987107625755, 4987107625762, 4901301368065, 4571138554759, 4901616009363, 4901616009370, 4582267392792, 4582267392808 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-Clinica AD &amp; NS TP are horizontally adjacent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301281511, 4903301281528, 4903301268963, 4903301268970, 4903301293781, 4903301297772 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301248880, 4903301281559, 4903301281566, 4903301281573, 4903301277057, 4903301277064, 4903301277071, 4903301297734, 4903301297741, 4903301297765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-Denthealth med TP are horizontally adjacent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301248958, 4903301248996, 4903301249023 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301249030, 4903301276081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-Systema products are horizontally adjacent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301277071, 4903301277064 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301293064, 4903301293101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301291701, 4903301099277, 4903301291695 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301282792, 4903301282785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-Systema &amp; DentHealth products are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301216803, 4903301231073, 4903301231097, 4903301293064 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4903301249078, 4903301249061, 4903301249023, 4903301248996, 4903301249016, 4903301248958, 4903301176657, 4903301276012, 4903301249047, 4903301275985, 4903301276005, 4903301249030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT-Clinica AD TP &amp; NS TP are VER ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT-Haguki Plus TP &amp; Haguki Plus Premium TP are VER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT-Nonio TP &amp; Nonio Plus TP are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT-DentHealth Non-Med &amp; Med TP are HOR ADJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT-Clinica AD TB &amp; NS TB are HOR ADJ</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +430,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -366,6 +484,27 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF3C3C3C"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -426,7 +565,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,6 +591,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,7 +680,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF3C3C3C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -536,33 +695,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ28"/>
+  <dimension ref="1:28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O4" activeCellId="0" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="1" sqref="A2 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="46.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="9.72"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.9744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.219387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.0204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="111.132653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="31.5765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.5459183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +2088,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>19</v>
@@ -1974,7 +2132,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>18</v>
@@ -2001,13 +2159,13 @@
         <v>22</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>26</v>
@@ -2021,7 +2179,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>18</v>
@@ -2051,10 +2209,10 @@
         <v>37</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>26</v>
@@ -2068,7 +2226,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>18</v>
@@ -2095,10 +2253,10 @@
         <v>22</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>25</v>
@@ -2115,7 +2273,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -2142,10 +2300,10 @@
         <v>22</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>32</v>
@@ -2162,7 +2320,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>18</v>
@@ -2189,10 +2347,10 @@
         <v>22</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>32</v>
@@ -2209,7 +2367,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>18</v>
@@ -2236,10 +2394,10 @@
         <v>22</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>32</v>
@@ -2256,13 +2414,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>40</v>
@@ -2303,13 +2461,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>40</v>
@@ -2350,13 +2508,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>40</v>
@@ -2397,13 +2555,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>40</v>
@@ -2444,13 +2602,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>40</v>
@@ -2491,13 +2649,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>40</v>
@@ -2518,13 +2676,13 @@
         <v>22</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>26</v>
@@ -2538,13 +2696,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>40</v>
@@ -2568,10 +2726,10 @@
         <v>37</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>26</v>
@@ -2585,13 +2743,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>40</v>
@@ -2612,10 +2770,10 @@
         <v>22</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>25</v>
@@ -2632,13 +2790,13 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>40</v>
@@ -2659,10 +2817,10 @@
         <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>32</v>
@@ -2679,13 +2837,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>40</v>
@@ -2706,10 +2864,10 @@
         <v>22</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>32</v>
@@ -2726,13 +2884,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>40</v>
@@ -2753,13 +2911,13 @@
         <v>22</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>26</v>
@@ -2773,13 +2931,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>40</v>
@@ -2800,10 +2958,10 @@
         <v>22</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="6" t="s">
@@ -2818,13 +2976,13 @@
         <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>40</v>
@@ -2845,10 +3003,10 @@
         <v>22</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="6" t="s">
@@ -2865,11 +3023,3005 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A2 C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="38.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="40.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="9.62755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="19.6275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="7" width="11.4285714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="8.93877551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="9.07142857142857"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.4642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="51.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="7" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="9"/>
+      <c r="N17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F25" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F26" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q36"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="1" sqref="A2 C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J14" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J16" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J17" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J18" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J19" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J20" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="9"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J21" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J22" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J23" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J24" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J25" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J26" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J27" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J28" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J29" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O29" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J30" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O30" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J31" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J32" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J33" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J34" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J35" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="J36" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="P36" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>